<commit_message>
PolynomialFlangeSegment: Implemented gap shapes other than sinusoidal
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBF8A6B-9223-4A56-8186-8E22BA2D8F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B206FEB4-A353-42D0-AC82-4EB5C26F6BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7080" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="36240" yWindow="4365" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5043,6 +5043,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5061,26 +5079,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -19861,32 +19861,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -19902,12 +19902,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19915,12 +19915,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19928,12 +19928,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19941,12 +19941,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19954,12 +19954,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -20007,112 +20007,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="s">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="s">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="s">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="171" t="s">
+      <c r="C17" s="171"/>
+      <c r="D17" s="174" t="s">
         <v>328</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20300,16 +20300,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24224,6 +24224,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="B4:G4"/>
@@ -24240,10 +24244,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="26" priority="5" stopIfTrue="1" operator="between">
@@ -24329,32 +24329,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -24370,12 +24370,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24383,12 +24383,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24396,12 +24396,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24409,12 +24409,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24422,12 +24422,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24475,117 +24475,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="167" t="str">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24773,16 +24773,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28659,6 +28659,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28672,13 +28679,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="between">
@@ -28764,32 +28764,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -28805,12 +28805,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28818,12 +28818,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28831,12 +28831,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28844,12 +28844,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28857,12 +28857,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28910,117 +28910,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="167" t="str">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29208,16 +29208,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33095,6 +33095,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33108,13 +33115,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="between">
@@ -33200,32 +33200,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -33241,12 +33241,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33254,12 +33254,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33267,12 +33267,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33280,12 +33280,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33293,12 +33293,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33346,117 +33346,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="167" t="str">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33644,16 +33644,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37531,6 +37531,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37544,13 +37551,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="between">
@@ -42020,12 +42020,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42282,17 +42281,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -42317,18 +42326,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reorganized history folders of validation
</commit_message>
<xml_diff>
--- a/tests/validation/BnB_ReferenceFlange-Results.xlsx
+++ b/tests/validation/BnB_ReferenceFlange-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B206FEB4-A353-42D0-AC82-4EB5C26F6BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228EA9BC-F735-4DB6-8925-83BA1191C0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36240" yWindow="4365" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="329">
   <si>
     <t>A</t>
   </si>
@@ -5043,6 +5043,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5070,17 +5079,8 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -19861,32 +19861,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -19902,12 +19902,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19915,12 +19915,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19928,12 +19928,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19941,12 +19941,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19954,12 +19954,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -20007,112 +20007,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="s">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="174" t="s">
+      <c r="C17" s="164"/>
+      <c r="D17" s="162" t="s">
         <v>328</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20300,16 +20300,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24224,16 +24224,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24244,6 +24234,16 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="26" priority="5" stopIfTrue="1" operator="between">
@@ -24329,32 +24329,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -24370,12 +24370,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24383,12 +24383,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24396,12 +24396,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24409,12 +24409,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24422,12 +24422,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24475,117 +24475,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173" t="str">
+      <c r="C17" s="164"/>
+      <c r="D17" s="163" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24773,16 +24773,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28659,13 +28659,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28679,6 +28672,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="between">
@@ -28764,32 +28764,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -28805,12 +28805,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28818,12 +28818,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28831,12 +28831,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28844,12 +28844,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28857,12 +28857,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28910,117 +28910,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173" t="str">
+      <c r="C17" s="164"/>
+      <c r="D17" s="163" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29208,16 +29208,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33095,13 +33095,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33115,6 +33108,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="between">
@@ -33200,32 +33200,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="167"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -33241,12 +33241,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="168"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="173"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33254,12 +33254,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="169"/>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="170"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33267,12 +33267,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169"/>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="170"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="172"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="172"/>
+      <c r="F7" s="172"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33280,12 +33280,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="169"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="169"/>
-      <c r="G8" s="170"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="172"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33293,12 +33293,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="169"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33346,117 +33346,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="164" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="171"/>
-      <c r="D13" s="173" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="163" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="173"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="164" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="173" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="163" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="171" t="s">
+      <c r="B15" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="173" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="163" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="173"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="173"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="173"/>
-      <c r="K15" s="173"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="171"/>
-      <c r="D16" s="173" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="163" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="173"/>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="173"/>
-      <c r="K16" s="173"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="171" t="s">
+      <c r="B17" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="173" t="str">
+      <c r="C17" s="164"/>
+      <c r="D17" s="163" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="173"/>
-      <c r="H17" s="173"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="173"/>
-      <c r="K17" s="173"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="171"/>
-      <c r="D18" s="172">
+      <c r="C18" s="164"/>
+      <c r="D18" s="174">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="174"/>
+      <c r="J18" s="174"/>
+      <c r="K18" s="174"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33644,16 +33644,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37531,13 +37531,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37551,6 +37544,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="between">
@@ -37587,8 +37587,8 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R120"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -40647,14 +40647,10 @@
         <f t="array" ref="E94">INDEX(N94:Q94,case_number)</f>
         <v>3595</v>
       </c>
-      <c r="F94" s="107" cm="1">
-        <f t="array" aca="1" ref="F94" ca="1">INDIRECT(sheet_name&amp;"!point2.Fs")</f>
-        <v>3595</v>
-      </c>
-      <c r="G94" s="118">
-        <f ca="1">(F94-E94)/E94</f>
-        <v>0</v>
-      </c>
+      <c r="F94" s="107" t="s">
+        <v>87</v>
+      </c>
+      <c r="G94" s="118"/>
       <c r="I94" s="151"/>
       <c r="K94" s="106">
         <f>K93+1</f>
@@ -42020,11 +42016,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42281,27 +42278,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -42326,9 +42313,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>